<commit_message>
Completed model CV, GridSearch and pipeline
</commit_message>
<xml_diff>
--- a/Proyecto 1/Etapa 1/Modelo_A/output.xlsx
+++ b/Proyecto 1/Etapa 1/Modelo_A/output.xlsx
@@ -2032,7 +2032,7 @@
         </is>
       </c>
       <c r="B160" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="161">
@@ -2222,7 +2222,7 @@
         </is>
       </c>
       <c r="B179" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="180">
@@ -3432,7 +3432,7 @@
         </is>
       </c>
       <c r="B300" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="301">
@@ -3772,7 +3772,7 @@
         </is>
       </c>
       <c r="B334" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="335">
@@ -3992,7 +3992,7 @@
         </is>
       </c>
       <c r="B356" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="357">
@@ -4942,7 +4942,7 @@
         </is>
       </c>
       <c r="B451" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="452">
@@ -6242,7 +6242,7 @@
         </is>
       </c>
       <c r="B581" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="582">
@@ -6782,7 +6782,7 @@
         </is>
       </c>
       <c r="B635" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="636">
@@ -7172,7 +7172,7 @@
         </is>
       </c>
       <c r="B674" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="675">

</xml_diff>